<commit_message>
modified: summary apis for coupon and campaign
</commit_message>
<xml_diff>
--- a/api/resources/excel/campaign_summary_workbook/campaign_summary_workbook.xlsx
+++ b/api/resources/excel/campaign_summary_workbook/campaign_summary_workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>campaign_summary_table</t>
   </si>
@@ -64,6 +64,12 @@
     <t>8ea2366a-391f-4a2a-99ea-f49d639bdcd1</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
     <t>total_redemption_count</t>
   </si>
   <si>
@@ -74,6 +80,15 @@
   </si>
   <si>
     <t>active_coupon_code_count</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>active, inactive</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
   <si>
     <t>created_at</t>
@@ -431,10 +446,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="K4" s="1">
-        <v>90.0</v>
       </c>
     </row>
     <row r="5">
@@ -445,38 +460,38 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1">
-        <v>900.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K6" s="1">
-        <v>13.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="K7" s="1">
+        <v>13.0</v>
       </c>
     </row>
     <row r="8">
@@ -489,8 +504,39 @@
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K8" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified: campaign summary mv, coupon item converter
</commit_message>
<xml_diff>
--- a/api/resources/excel/campaign_summary_workbook/campaign_summary_workbook.xlsx
+++ b/api/resources/excel/campaign_summary_workbook/campaign_summary_workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>campaign_summary_table</t>
   </si>
@@ -70,10 +70,16 @@
     <t>default</t>
   </si>
   <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
     <t>total_redemption_count</t>
-  </si>
-  <si>
-    <t>number</t>
   </si>
   <si>
     <t>total_redemption_amount</t>
@@ -457,69 +463,69 @@
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="1">
-        <v>90.0</v>
+        <v>1500000.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K6" s="1">
-        <v>900.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="1">
-        <v>13.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="K8" s="1">
+        <v>13.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>27</v>
@@ -536,7 +542,21 @@
         <v>14</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>